<commit_message>
ActivityTests:  Updated waits on ActivityTests; Updated user stories
</commit_message>
<xml_diff>
--- a/LogBox20220513/resources/testDataInput/MDTMeetings.xlsx
+++ b/LogBox20220513/resources/testDataInput/MDTMeetings.xlsx
@@ -1,34 +1,24 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="25225"/>
-  <workbookPr defaultThemeVersion="166925"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="25225"/>
+  <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Yolande\Downloads\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\autoProgram\LogBoxPremiumAutomation\LogBox20220513\resources\testDataInput\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{E446FC13-9C55-4AD0-98D9-58E19312264E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{56304CB5-0633-40B2-BEAB-47C8A42DE466}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="6000" yWindow="2940" windowWidth="13632" windowHeight="7908" xr2:uid="{3AC9DFFD-ED36-4752-85FF-53C6F5CD71F7}"/>
+    <workbookView xWindow="1152" yWindow="1152" windowWidth="17280" windowHeight="9072" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="191029"/>
+  <calcPr calcId="162913"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
-    </ext>
-    <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
-      <xcalcf:calcFeatures>
-        <xcalcf:feature name="microsoft.com:RD"/>
-        <xcalcf:feature name="microsoft.com:Single"/>
-        <xcalcf:feature name="microsoft.com:FV"/>
-        <xcalcf:feature name="microsoft.com:CNMTM"/>
-        <xcalcf:feature name="microsoft.com:LET_WF"/>
-        <xcalcf:feature name="microsoft.com:LAMBDA_WF"/>
-      </xcalcf:calcFeatures>
     </ext>
   </extLst>
 </workbook>
@@ -124,7 +114,7 @@
         <a:srgbClr val="E7E6E6"/>
       </a:lt2>
       <a:accent1>
-        <a:srgbClr val="4472C4"/>
+        <a:srgbClr val="5B9BD5"/>
       </a:accent1>
       <a:accent2>
         <a:srgbClr val="ED7D31"/>
@@ -136,7 +126,7 @@
         <a:srgbClr val="FFC000"/>
       </a:accent4>
       <a:accent5>
-        <a:srgbClr val="5B9BD5"/>
+        <a:srgbClr val="4472C4"/>
       </a:accent5>
       <a:accent6>
         <a:srgbClr val="70AD47"/>
@@ -183,23 +173,6 @@
         <a:font script="Viet" typeface="Times New Roman"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
         <a:font script="Geor" typeface="Sylfaen"/>
-        <a:font script="Armn" typeface="Arial"/>
-        <a:font script="Bugi" typeface="Leelawadee UI"/>
-        <a:font script="Bopo" typeface="Microsoft JhengHei"/>
-        <a:font script="Java" typeface="Javanese Text"/>
-        <a:font script="Lisu" typeface="Segoe UI"/>
-        <a:font script="Mymr" typeface="Myanmar Text"/>
-        <a:font script="Nkoo" typeface="Ebrima"/>
-        <a:font script="Olck" typeface="Nirmala UI"/>
-        <a:font script="Osma" typeface="Ebrima"/>
-        <a:font script="Phag" typeface="Phagspa"/>
-        <a:font script="Syrn" typeface="Estrangelo Edessa"/>
-        <a:font script="Syrj" typeface="Estrangelo Edessa"/>
-        <a:font script="Syre" typeface="Estrangelo Edessa"/>
-        <a:font script="Sora" typeface="Nirmala UI"/>
-        <a:font script="Tale" typeface="Microsoft Tai Le"/>
-        <a:font script="Talu" typeface="Microsoft New Tai Lue"/>
-        <a:font script="Tfng" typeface="Ebrima"/>
       </a:majorFont>
       <a:minorFont>
         <a:latin typeface="Calibri" panose="020F0502020204030204"/>
@@ -235,23 +208,6 @@
         <a:font script="Viet" typeface="Arial"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
         <a:font script="Geor" typeface="Sylfaen"/>
-        <a:font script="Armn" typeface="Arial"/>
-        <a:font script="Bugi" typeface="Leelawadee UI"/>
-        <a:font script="Bopo" typeface="Microsoft JhengHei"/>
-        <a:font script="Java" typeface="Javanese Text"/>
-        <a:font script="Lisu" typeface="Segoe UI"/>
-        <a:font script="Mymr" typeface="Myanmar Text"/>
-        <a:font script="Nkoo" typeface="Ebrima"/>
-        <a:font script="Olck" typeface="Nirmala UI"/>
-        <a:font script="Osma" typeface="Ebrima"/>
-        <a:font script="Phag" typeface="Phagspa"/>
-        <a:font script="Syrn" typeface="Estrangelo Edessa"/>
-        <a:font script="Syrj" typeface="Estrangelo Edessa"/>
-        <a:font script="Syre" typeface="Estrangelo Edessa"/>
-        <a:font script="Sora" typeface="Nirmala UI"/>
-        <a:font script="Tale" typeface="Microsoft Tai Le"/>
-        <a:font script="Talu" typeface="Microsoft New Tai Lue"/>
-        <a:font script="Tfng" typeface="Ebrima"/>
       </a:minorFont>
     </a:fontScheme>
     <a:fmtScheme name="Office">
@@ -403,11 +359,11 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{9E451F3C-4316-4CE8-B20E-0D03B03967F7}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:C2"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C2" sqref="C2"/>
+      <selection sqref="A1:C2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>

</xml_diff>